<commit_message>
salvando antes das mudanças
</commit_message>
<xml_diff>
--- a/data/teacher/Allan Cupertino.xlsx
+++ b/data/teacher/Allan Cupertino.xlsx
@@ -985,27 +985,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>[-, 'ELM-2NA-Instalções Elétricas']</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>ELM-2NA-Máquinas Elétricas</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>[-, 'ELM-2NA-Instalções Elétricas']</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>['ELM-2NA-Instalções Elétricas', -]</t>
         </is>
       </c>
     </row>
@@ -1017,27 +1017,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>[-, 'ELM-2NA-Instalções Elétricas']</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>ELM-2NA-Máquinas Elétricas</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>[-, 'ELM-2NA-Instalções Elétricas']</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>['ELM-2NA-Instalções Elétricas', -]</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>['ELM-2NA-Instalções Elétricas', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">

</xml_diff>